<commit_message>
rough runnable code for backprojection_MCNP_Gammas
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artao\Desktop\Master\NERS599 independent reseach 25WN\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F6CEE5-0AAA-4433-BE50-070ED0A1F5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F132DC-D45A-4D5D-801E-4627250D6F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="工作表1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -431,7 +432,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -48970,4 +48973,519 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB49537-48BD-4399-A9D7-4BC3E49AFDE5}">
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>-2.5</v>
+      </c>
+      <c r="B1">
+        <v>0.58713351915171197</v>
+      </c>
+      <c r="C1">
+        <v>0.48291820425854498</v>
+      </c>
+      <c r="D1">
+        <v>0.43939861829540899</v>
+      </c>
+      <c r="E1">
+        <v>0.39721456856431298</v>
+      </c>
+      <c r="F1">
+        <v>0.36983940712879998</v>
+      </c>
+      <c r="G1">
+        <v>0.342752590385347</v>
+      </c>
+      <c r="H1">
+        <v>0.32228974774039199</v>
+      </c>
+      <c r="I1">
+        <v>0.30425488535119199</v>
+      </c>
+      <c r="J1">
+        <v>0.28844913104541398</v>
+      </c>
+      <c r="K1">
+        <v>0.27234731623875102</v>
+      </c>
+      <c r="L1">
+        <v>0.26286140635437599</v>
+      </c>
+      <c r="M1">
+        <v>0.25254163390884499</v>
+      </c>
+      <c r="N1">
+        <v>0.24503555307861599</v>
+      </c>
+      <c r="O1">
+        <v>0.23917541804407799</v>
+      </c>
+      <c r="P1">
+        <v>0.23142241571064301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>-2</v>
+      </c>
+      <c r="B2">
+        <v>0.51089037336028198</v>
+      </c>
+      <c r="C2">
+        <v>0.42020810195367903</v>
+      </c>
+      <c r="D2">
+        <v>0.38233982021545598</v>
+      </c>
+      <c r="E2">
+        <v>0.34563364655310802</v>
+      </c>
+      <c r="F2">
+        <v>0.32181332972501497</v>
+      </c>
+      <c r="G2">
+        <v>0.29824391413586898</v>
+      </c>
+      <c r="H2">
+        <v>0.28043830607929299</v>
+      </c>
+      <c r="I2">
+        <v>0.26474538908686501</v>
+      </c>
+      <c r="J2">
+        <v>0.25099211584471298</v>
+      </c>
+      <c r="K2">
+        <v>0.236981227503268</v>
+      </c>
+      <c r="L2">
+        <v>0.22872712535374001</v>
+      </c>
+      <c r="M2">
+        <v>0.219747443176323</v>
+      </c>
+      <c r="N2">
+        <v>0.213216076267875</v>
+      </c>
+      <c r="O2">
+        <v>0.208116918277266</v>
+      </c>
+      <c r="P2">
+        <v>0.20137069424543999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>-1.5</v>
+      </c>
+      <c r="B3">
+        <v>0.45443314139090901</v>
+      </c>
+      <c r="C3">
+        <v>0.37377194358300903</v>
+      </c>
+      <c r="D3">
+        <v>0.34008839202929603</v>
+      </c>
+      <c r="E3">
+        <v>0.30743852686133799</v>
+      </c>
+      <c r="F3">
+        <v>0.28625053434952102</v>
+      </c>
+      <c r="G3">
+        <v>0.26528571660109501</v>
+      </c>
+      <c r="H3">
+        <v>0.24944776226599</v>
+      </c>
+      <c r="I3">
+        <v>0.23548903072922001</v>
+      </c>
+      <c r="J3">
+        <v>0.223255597707708</v>
+      </c>
+      <c r="K3">
+        <v>0.21079301799456501</v>
+      </c>
+      <c r="L3">
+        <v>0.203451056265084</v>
+      </c>
+      <c r="M3">
+        <v>0.195463696562579</v>
+      </c>
+      <c r="N3">
+        <v>0.189654094862197</v>
+      </c>
+      <c r="O3">
+        <v>0.18511843221332</v>
+      </c>
+      <c r="P3">
+        <v>0.17911771671902499</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>-1</v>
+      </c>
+      <c r="B4">
+        <v>0.41724313482505099</v>
+      </c>
+      <c r="C4">
+        <v>0.34318310714066902</v>
+      </c>
+      <c r="D4">
+        <v>0.31225615802050599</v>
+      </c>
+      <c r="E4">
+        <v>0.28227830021595002</v>
+      </c>
+      <c r="F4">
+        <v>0.26282429563076198</v>
+      </c>
+      <c r="G4">
+        <v>0.24357520158006099</v>
+      </c>
+      <c r="H4">
+        <v>0.229033397485912</v>
+      </c>
+      <c r="I4">
+        <v>0.216217023911668</v>
+      </c>
+      <c r="J4">
+        <v>0.20498475346601999</v>
+      </c>
+      <c r="K4">
+        <v>0.193542089289716</v>
+      </c>
+      <c r="L4">
+        <v>0.18680098075525101</v>
+      </c>
+      <c r="M4">
+        <v>0.17946729247924201</v>
+      </c>
+      <c r="N4">
+        <v>0.17413313833253299</v>
+      </c>
+      <c r="O4">
+        <v>0.16996866631287799</v>
+      </c>
+      <c r="P4">
+        <v>0.16445903878797999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>-0.5</v>
+      </c>
+      <c r="B5">
+        <v>0.41435816817981502</v>
+      </c>
+      <c r="C5">
+        <v>0.34081021772758202</v>
+      </c>
+      <c r="D5">
+        <v>0.31009710847488198</v>
+      </c>
+      <c r="E5">
+        <v>0.28032652818466602</v>
+      </c>
+      <c r="F5">
+        <v>0.26100703546956</v>
+      </c>
+      <c r="G5">
+        <v>0.241891036465014</v>
+      </c>
+      <c r="H5">
+        <v>0.227449779548929</v>
+      </c>
+      <c r="I5">
+        <v>0.21472202291571699</v>
+      </c>
+      <c r="J5">
+        <v>0.20356741636164899</v>
+      </c>
+      <c r="K5">
+        <v>0.19220387081361301</v>
+      </c>
+      <c r="L5">
+        <v>0.18550937268840401</v>
+      </c>
+      <c r="M5">
+        <v>0.178226392127627</v>
+      </c>
+      <c r="N5">
+        <v>0.17292912020979001</v>
+      </c>
+      <c r="O5">
+        <v>0.16879344282297301</v>
+      </c>
+      <c r="P5">
+        <v>0.16332191081196301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0.44074518254712702</v>
+      </c>
+      <c r="C6">
+        <v>0.36251357680750301</v>
+      </c>
+      <c r="D6">
+        <v>0.32984460589367998</v>
+      </c>
+      <c r="E6">
+        <v>0.29817818574759197</v>
+      </c>
+      <c r="F6">
+        <v>0.27762839574142101</v>
+      </c>
+      <c r="G6">
+        <v>0.25729505826230298</v>
+      </c>
+      <c r="H6">
+        <v>0.24193415818966801</v>
+      </c>
+      <c r="I6">
+        <v>0.228395876935645</v>
+      </c>
+      <c r="J6">
+        <v>0.216530926563096</v>
+      </c>
+      <c r="K6">
+        <v>0.20444373161541801</v>
+      </c>
+      <c r="L6">
+        <v>0.19732291676285299</v>
+      </c>
+      <c r="M6">
+        <v>0.189576143938638</v>
+      </c>
+      <c r="N6">
+        <v>0.183941532972273</v>
+      </c>
+      <c r="O6">
+        <v>0.17954248880037799</v>
+      </c>
+      <c r="P6">
+        <v>0.17372252056951401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.5</v>
+      </c>
+      <c r="B7">
+        <v>0.49712674385147798</v>
+      </c>
+      <c r="C7">
+        <v>0.408887495942163</v>
+      </c>
+      <c r="D7">
+        <v>0.37203940371456201</v>
+      </c>
+      <c r="E7">
+        <v>0.33632211181886601</v>
+      </c>
+      <c r="F7">
+        <v>0.31314352564905101</v>
+      </c>
+      <c r="G7">
+        <v>0.29020908131953999</v>
+      </c>
+      <c r="H7">
+        <v>0.27288316480786001</v>
+      </c>
+      <c r="I7">
+        <v>0.25761302245879703</v>
+      </c>
+      <c r="J7">
+        <v>0.244230268935373</v>
+      </c>
+      <c r="K7">
+        <v>0.230596840585888</v>
+      </c>
+      <c r="L7">
+        <v>0.222565107871836</v>
+      </c>
+      <c r="M7">
+        <v>0.21382734260074801</v>
+      </c>
+      <c r="N7">
+        <v>0.20747193382148299</v>
+      </c>
+      <c r="O7">
+        <v>0.20251014957101299</v>
+      </c>
+      <c r="P7">
+        <v>0.195945672021406</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0.56846877102151405</v>
+      </c>
+      <c r="C8">
+        <v>0.46756642079539701</v>
+      </c>
+      <c r="D8">
+        <v>0.42543030568554502</v>
+      </c>
+      <c r="E8">
+        <v>0.38458727062600201</v>
+      </c>
+      <c r="F8">
+        <v>0.35808235501456498</v>
+      </c>
+      <c r="G8">
+        <v>0.33185661772863601</v>
+      </c>
+      <c r="H8">
+        <v>0.31204428095932601</v>
+      </c>
+      <c r="I8">
+        <v>0.29458273988985401</v>
+      </c>
+      <c r="J8">
+        <v>0.27927944441754798</v>
+      </c>
+      <c r="K8">
+        <v>0.26368950009349701</v>
+      </c>
+      <c r="L8">
+        <v>0.25450514362585303</v>
+      </c>
+      <c r="M8">
+        <v>0.24451343276627099</v>
+      </c>
+      <c r="N8">
+        <v>0.23724596735071601</v>
+      </c>
+      <c r="O8">
+        <v>0.23157212374880901</v>
+      </c>
+      <c r="P8">
+        <v>0.22406558636940299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1.5</v>
+      </c>
+      <c r="B9">
+        <v>0.66067490545242202</v>
+      </c>
+      <c r="C9">
+        <v>0.54340610531099098</v>
+      </c>
+      <c r="D9">
+        <v>0.49443547528621501</v>
+      </c>
+      <c r="E9">
+        <v>0.44696766403272298</v>
+      </c>
+      <c r="F9">
+        <v>0.41616362780722599</v>
+      </c>
+      <c r="G9">
+        <v>0.38568405287707502</v>
+      </c>
+      <c r="H9">
+        <v>0.36265813766569999</v>
+      </c>
+      <c r="I9">
+        <v>0.34236431928338801</v>
+      </c>
+      <c r="J9">
+        <v>0.32457881583153098</v>
+      </c>
+      <c r="K9">
+        <v>0.30646016883216598</v>
+      </c>
+      <c r="L9">
+        <v>0.29578610167101399</v>
+      </c>
+      <c r="M9">
+        <v>0.28417372652576101</v>
+      </c>
+      <c r="N9">
+        <v>0.27572747183058699</v>
+      </c>
+      <c r="O9">
+        <v>0.26913332580827098</v>
+      </c>
+      <c r="P9">
+        <v>0.26040922146652801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0.72383687498744997</v>
+      </c>
+      <c r="C10">
+        <v>0.59535692043283495</v>
+      </c>
+      <c r="D10">
+        <v>0.54170459080631905</v>
+      </c>
+      <c r="E10">
+        <v>0.489698752720653</v>
+      </c>
+      <c r="F10">
+        <v>0.45594978309209599</v>
+      </c>
+      <c r="G10">
+        <v>0.42255629397012201</v>
+      </c>
+      <c r="H10">
+        <v>0.39732905077868602</v>
+      </c>
+      <c r="I10">
+        <v>0.37509509886347497</v>
+      </c>
+      <c r="J10">
+        <v>0.35560926228571799</v>
+      </c>
+      <c r="K10">
+        <v>0.33575843290687302</v>
+      </c>
+      <c r="L10">
+        <v>0.32406390152150999</v>
+      </c>
+      <c r="M10">
+        <v>0.31134135785146499</v>
+      </c>
+      <c r="N10">
+        <v>0.30208762268845502</v>
+      </c>
+      <c r="O10">
+        <v>0.29486306184830202</v>
+      </c>
+      <c r="P10">
+        <v>0.28530491400330699</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>